<commit_message>
This is a squashed commit that ignores all previous history.
All the relevant code in this commit is a complete rewrite of previous work and the history of developing this new code is not useful but it is still maintained here: https://github.com/ShahimEssaid/comp-loinc/tree/dev-se in case it might be useful.  Also see the main-old branch for one previous PR that is no longer applicable to the new code, and was left out of this new "main" history.

There will likely be more Git history rewrites to remove large files that were committed in the past and would be good to remove to reduce the overall size of the repository. This will have to rewrite the history of "main" and have it force pushed but it will not likely affect anything you do that is based on the new implementation. It will only remove non-code files from the history.
</commit_message>
<xml_diff>
--- a/project/excel/comp_loinc.xlsx
+++ b/project/excel/comp_loinc.xlsx
@@ -8,17 +8,17 @@
   </bookViews>
   <sheets>
     <sheet name="Thing" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="CodeBySystem" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="CodeByComponent" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="LoincCodeClass" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="PartClass" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="ComponentClass" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="SystemClass" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="MethodClass" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="TimeClass" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="PropertyClass" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="ScaleClass" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="LoincCodeOntology" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="Loinc" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="PartClass" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="ComponentClass" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="SystemClass" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="MethodClass" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="TimeClass" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="PropertyClass" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="ScaleClass" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="LoincCodeClass" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="LoincCodeClassIntersection" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="LoincCodeClassNonIntersection" sheetId="12" state="visible" r:id="rId12"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,6 +446,16 @@
       <c r="C1" t="inlineStr">
         <is>
           <t>description</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>subClassOf</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>equivalentClasses</t>
         </is>
       </c>
     </row>
@@ -460,7 +470,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:AF1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,32 +481,162 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>loinc_number</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>long_common_name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>formal_name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>short_name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>status</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>loinc_class</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>loinc_class_type</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>has_component</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>has_property</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>has_time</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>has_system</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>has_scale</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>has_method</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>has_component_analyte</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>has_component_challenge</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>has_component_count</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>has_component_adjustment</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>has_time_core</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>has_time_modifier</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>has_system_core</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>has_system_super_system</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>semantic_analyte_gene</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>syntax_analyte_core</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>syntax_analyte_suffix</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>syntax_analyte_divisor</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>syntax_analyte_divisor_suffix</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>syntax_analyte_numerator</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>label</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
           <t>subClassOf</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>part_number</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>part_type</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>label</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>description</t>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>equivalentClasses</t>
         </is>
       </c>
     </row>
@@ -511,7 +651,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:AF1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -522,32 +662,162 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>loinc_number</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>long_common_name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>formal_name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>short_name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>status</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>loinc_class</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>loinc_class_type</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>has_component</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>has_property</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>has_time</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>has_system</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>has_scale</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>has_method</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>has_component_analyte</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>has_component_challenge</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>has_component_count</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>has_component_adjustment</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>has_time_core</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>has_time_modifier</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>has_system_core</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>has_system_super_system</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>semantic_analyte_gene</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>syntax_analyte_core</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>syntax_analyte_suffix</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>syntax_analyte_divisor</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>syntax_analyte_divisor_suffix</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>syntax_analyte_numerator</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>label</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
           <t>subClassOf</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>part_number</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>part_type</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>label</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>description</t>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>equivalentClasses</t>
         </is>
       </c>
     </row>
@@ -562,7 +832,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:AF1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -573,17 +843,162 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>component_class_set</t>
+          <t>loinc_number</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>system_class_set</t>
+          <t>long_common_name</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>code_class_set</t>
+          <t>formal_name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>short_name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>status</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>loinc_class</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>loinc_class_type</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>has_component</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>has_property</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>has_time</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>has_system</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>has_scale</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>has_method</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>has_component_analyte</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>has_component_challenge</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>has_component_count</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>has_component_adjustment</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>has_time_core</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>has_time_modifier</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>has_system_core</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>has_system_super_system</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>semantic_analyte_gene</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>syntax_analyte_core</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>syntax_analyte_suffix</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>syntax_analyte_divisor</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>syntax_analyte_divisor_suffix</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>syntax_analyte_numerator</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>label</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>subClassOf</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>equivalentClasses</t>
         </is>
       </c>
     </row>
@@ -598,7 +1013,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -609,22 +1024,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>has_system</t>
+          <t>codes</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>label</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>description</t>
+          <t>parts</t>
         </is>
       </c>
     </row>
@@ -639,7 +1044,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -650,22 +1055,47 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>has_component</t>
+          <t>subClassOf</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
+          <t>part_number</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>part_type</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>part_name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>part_display_name</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>label</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>description</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>equivalentClasses</t>
         </is>
       </c>
     </row>
@@ -680,7 +1110,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -696,72 +1126,42 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>formal_name</t>
+          <t>part_number</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>loinc_number</t>
+          <t>part_type</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>status</t>
+          <t>part_name</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>short_name</t>
+          <t>part_display_name</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>long_common_name</t>
+          <t>id</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>has_component</t>
+          <t>label</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>has_property</t>
+          <t>description</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>has_system</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>has_method</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>has_scale</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>has_time</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>label</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>description</t>
+          <t>equivalentClasses</t>
         </is>
       </c>
     </row>
@@ -776,7 +1176,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -802,17 +1202,32 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
+          <t>part_name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>part_display_name</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>label</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>description</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>equivalentClasses</t>
         </is>
       </c>
     </row>
@@ -827,7 +1242,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -853,17 +1268,32 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
+          <t>part_name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>part_display_name</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>label</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>description</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>equivalentClasses</t>
         </is>
       </c>
     </row>
@@ -878,7 +1308,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -904,17 +1334,32 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
+          <t>part_name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>part_display_name</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>label</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>description</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>equivalentClasses</t>
         </is>
       </c>
     </row>
@@ -929,7 +1374,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -955,17 +1400,32 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
+          <t>part_name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>part_display_name</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>label</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>description</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>equivalentClasses</t>
         </is>
       </c>
     </row>
@@ -980,7 +1440,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1006,17 +1466,32 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
+          <t>part_name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>part_display_name</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>label</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>description</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>equivalentClasses</t>
         </is>
       </c>
     </row>

</xml_diff>